<commit_message>
Geração do relatório implementado.
Aprimorado o salvamento de alinhamentos, bem como indicação de campos que utilizam vocabulário controlado.
</commit_message>
<xml_diff>
--- a/data/fontes/Base_Regex.xlsx
+++ b/data/fontes/Base_Regex.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeil\Desktop\Mestrado\Qualidade dados\Planilhas de apoio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samantha\Desktop\Qualidade dados\Planilhas de apoio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBA8C32-C5E8-4E19-8DD1-E88CA444867A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB8B343-98C6-4040-87CB-199FE26E9C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1035" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId1"/>
     <sheet name="tabela resumo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t>Nome da Regra</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Abreviar unidades métricas de acordo com o Sistema Internacional (m, cm, mm, g, kg, kb, Mb, Gb)</t>
   </si>
   <si>
-    <t>Measurements, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso, Measurements_espessura</t>
-  </si>
-  <si>
     <t>([0-9]{1,}([,\.][0-9 ]{1,})*) ((m|M|cm|CM|Cm|g|G|kg|KG|Kg)+)|(\((m|M|cm|CM|Cm|g|G|kg|KG|Kg)\): ([0-9]{1,}([,\.][0-9 ]{1,}))*)</t>
   </si>
   <si>
@@ -70,27 +67,18 @@
     <t>Anos com menos que 4 digitos, inserir 0 a esquerda</t>
   </si>
   <si>
-    <t xml:space="preserve">Date, </t>
-  </si>
-  <si>
     <t>([0-9]{4})</t>
   </si>
   <si>
     <t>Capitalize as inicais de nomes próprios e da primeira palavra, para outros termos use letras minúsculas</t>
   </si>
   <si>
-    <t xml:space="preserve">Creation Location, Date, Description, Materials and Techniques, Other Descriptive Notes, Title, Work Type, </t>
-  </si>
-  <si>
     <t>^([A-Z0-9]){1}(.)*</t>
   </si>
   <si>
     <t>Evitar abreviações</t>
   </si>
   <si>
-    <t xml:space="preserve">Class, Creation Location, Creator, Date, Description, Materials and Techniques, Other Descriptive Notes, Title, Work Type, </t>
-  </si>
-  <si>
     <t>(([a-zA-Z\u00C0-\u00FF ][\.]))*</t>
   </si>
   <si>
@@ -100,9 +88,6 @@
     <t>Fazer uso de vocabulário controlado</t>
   </si>
   <si>
-    <t>Class, Creation Location, Creator, Inscription, Location, Materials and Techniques, Measurements, Physical Description, Work Type, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso, Measurements_espessura</t>
-  </si>
-  <si>
     <t>Não se aplica</t>
   </si>
   <si>
@@ -115,9 +100,6 @@
     <t>Não pode ficar vazio</t>
   </si>
   <si>
-    <t xml:space="preserve">Creation Location, Creator, Date, Title, </t>
-  </si>
-  <si>
     <t>(.{1,})*</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t>Não usar pontuação, exceto hífen</t>
   </si>
   <si>
-    <t xml:space="preserve">Work Type, </t>
-  </si>
-  <si>
     <t>[a-zA-Z\u00C0-\u00FF 0-9\-\—\–]*</t>
   </si>
   <si>
@@ -145,9 +124,6 @@
     <t>Não utilizar artigos</t>
   </si>
   <si>
-    <t xml:space="preserve">Title, </t>
-  </si>
-  <si>
     <t>( o |^o | os |^os | a |^a | as |^as | uma |^uma | um |^um | uns |^uns | uma |^uma | umas |^umas | O |^O | Os |^Os | A |^A | As |^As | Uma |^Uma | Um |^Um | Uns |^Uns | Uma |^Uma | Umas |^Umas)</t>
   </si>
   <si>
@@ -166,15 +142,9 @@
     <t>Usar o mesmo idioma do catálogo</t>
   </si>
   <si>
-    <t xml:space="preserve">Creation Location, Creator, Date, Description, Materials and Techniques, Other Descriptive Notes, Title, Work Type, </t>
-  </si>
-  <si>
     <t>Usar singular</t>
   </si>
   <si>
-    <t xml:space="preserve">Class, Materials and Techniques, Work Type, </t>
-  </si>
-  <si>
     <t>(.[s] |.[s]$)</t>
   </si>
   <si>
@@ -199,28 +169,55 @@
     <t>regex</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Creation Location, Date, Description, Materials and Techniques, Other Descriptive Notes, Title, Work Type</t>
-  </si>
-  <si>
-    <t>Class, Creation Location, Creator, Date, Description, Materials and Techniques, Other Descriptive Notes, Title, Work Type</t>
-  </si>
-  <si>
-    <t>Creation Location, Creator, Date, Title</t>
-  </si>
-  <si>
-    <t>Work Type</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Creation Location, Creator, Date, Description, Materials and Techniques, Other Descriptive Notes, Title, Work Type</t>
-  </si>
-  <si>
-    <t>Class, Materials and Techniques, Work Type</t>
+    <t>,Date,</t>
+  </si>
+  <si>
+    <t>,Creation Location,Date,Description,Location,Materials and Techniques,Other Descriptive Notes,Title,Work Type</t>
+  </si>
+  <si>
+    <t>Class,Creation Location,Creator,Description,Location,Materials and Techniques,Other Descriptive Notes,Title,Work Type</t>
+  </si>
+  <si>
+    <t>,Work Type</t>
+  </si>
+  <si>
+    <t>,Title,</t>
+  </si>
+  <si>
+    <t>,Creation Location,Date,Description,Location,Materials and Techniques,Other Descriptive Notes,Work Type</t>
+  </si>
+  <si>
+    <t>Class,Materials and Techniques,Work Type</t>
+  </si>
+  <si>
+    <t>,Measurements, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso, Measurements_espessura,</t>
+  </si>
+  <si>
+    <t>Class,Creation Location,Creator,Inscription,Location,Materials and Techniques,Measurements, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso, Measurements_espessura,Physical Description,Work Type</t>
+  </si>
+  <si>
+    <t>Class,Creator,Inscription,Materials and Techniques,Measurements, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso, Measurements_espessura,Work Type</t>
+  </si>
+  <si>
+    <t>Class,Creator,Inscription,Materials and Techniques,Measurements, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso,Measurements_espessura,Work Type,Title,Date,Location,</t>
+  </si>
+  <si>
+    <t>,Creation Location,Date,Description,Location,Materials and Techniques,Other Descriptive Notes,Title,Work Type,</t>
+  </si>
+  <si>
+    <t>Class,Creation Location,Creator,Description,Location,Materials and Techniques,Other Descriptive Notes,Title,Work Type,</t>
+  </si>
+  <si>
+    <t>Class,Creation Location,Creator,Inscription,Location,Materials and Techniques,Measurements, Measurements_Altura, Measurements_Largura, Measurements_profundidade, Measurements_diametro, Measurements_peso, Measurements_espessura,Physical Description,Work Type,Inscription,Location,</t>
+  </si>
+  <si>
+    <t>,Work Type,</t>
+  </si>
+  <si>
+    <t>,Creation Location,Date,Description,Location,Materials and Techniques,Other Descriptive Notes,Work Type,</t>
+  </si>
+  <si>
+    <t>Class,Materials and Techniques,Work Type,</t>
   </si>
 </sst>
 </file>
@@ -297,22 +294,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -641,331 +631,331 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1593F18-74CB-49B4-852F-BA4F8ACE44E1}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>21</v>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>8</v>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D10">
+      <c r="B14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11">
+      <c r="B15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12">
+      <c r="B17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <autoFilter ref="A1:E18" xr:uid="{A1593F18-74CB-49B4-852F-BA4F8ACE44E1}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -973,213 +963,213 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1768680F-ADC9-4FEC-9480-0C381EAC24E4}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:C18"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="B9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="11" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="B10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="C15" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="C16" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="C17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="11" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="B18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Página de relatório final
</commit_message>
<xml_diff>
--- a/data/fontes/Base_Regex.xlsx
+++ b/data/fontes/Base_Regex.xlsx
@@ -1,35 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samantha\Desktop\Qualidade dados\Planilhas de apoio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeil\Documents\GitHub\DataQ-culture\data\fontes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB8B343-98C6-4040-87CB-199FE26E9C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA8C7B-C62E-4837-9A12-48F14FF32073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4440" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="3" r:id="rId1"/>
     <sheet name="tabela resumo" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1 bkp" sheetId="4" r:id="rId3"/>
+    <sheet name="tabela resumo bkp" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Planilha1 bkp'!$A$1:$E$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tabela resumo'!$A$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'tabela resumo bkp'!$A$1:$C$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="74">
   <si>
     <t>Nome da Regra</t>
   </si>
@@ -218,6 +214,48 @@
   </si>
   <si>
     <t>Class,Materials and Techniques,Work Type,</t>
+  </si>
+  <si>
+    <t>(?i)\b\d+(?:\.\d+)?\s*(?:m|cm|g|kg|B|KB|MB|GB|TB)\b</t>
+  </si>
+  <si>
+    <t>\b\d{4}\b</t>
+  </si>
+  <si>
+    <t>[A-ZÁÉÍÓÚÜÑ][A-Za-z0-9áéíóúüñ]*\.</t>
+  </si>
+  <si>
+    <t>\d+[,.]\d{2}\b</t>
+  </si>
+  <si>
+    <t>^$</t>
+  </si>
+  <si>
+    <t>.+</t>
+  </si>
+  <si>
+    <t>[A-Z]</t>
+  </si>
+  <si>
+    <t>^[a-zA-Z\u00C0-\u00FF 0-9\-\—\–]*$</t>
+  </si>
+  <si>
+    <t>[\']+</t>
+  </si>
+  <si>
+    <t>\b(?:o(s)?|a(s)?|um(a)?(s)?|uns)\b|\b(?:O(s)?|A(s)?|Um(a)?(s)?|Uns)\b</t>
+  </si>
+  <si>
+    <t>(?P&lt;hours&gt;0?[0-9]|1[0-9]|2[0-3]):(?P&lt;minutes&gt;60|[0-5][0-9]):(?P&lt;seconds&gt;60|[0-5][0-9])</t>
+  </si>
+  <si>
+    <t>(?:([0-9]{1,2})([/.\-])([0-9]{1,2})\2([0-9]{4}))</t>
+  </si>
+  <si>
+    <t>\b\w+[sS]\b</t>
+  </si>
+  <si>
+    <t>\b\d{4}\s*-\s*\d{4}\b</t>
   </si>
 </sst>
 </file>
@@ -296,20 +334,15 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,6 +350,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,8 +676,578 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1593F18-74CB-49B4-852F-BA4F8ACE44E1}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E18" xr:uid="{A1593F18-74CB-49B4-852F-BA4F8ACE44E1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
+      <sortCondition ref="A1:A18"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1768680F-ADC9-4FEC-9480-0C381EAC24E4}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6" t="str">
+        <f>VLOOKUP(A2,Planilha1!A:C,3,0)</f>
+        <v>(?i)\b\d+(?:\.\d+)?\s*(?:m|cm|g|kg|B|KB|MB|GB|TB)\b</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f>VLOOKUP(A3,Planilha1!A:C,3,0)</f>
+        <v>\b\d{4}\b</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="6" t="str">
+        <f>VLOOKUP(A4,Planilha1!A:C,3,0)</f>
+        <v>^([A-Z0-9]){1}(.)*</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="str">
+        <f>VLOOKUP(A5,Planilha1!A:C,3,0)</f>
+        <v>[A-ZÁÉÍÓÚÜÑ][A-Za-z0-9áéíóúüñ]*\.</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="6" t="str">
+        <f>VLOOKUP(A6,Planilha1!A:C,3,0)</f>
+        <v>Não se aplica</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f>VLOOKUP(A7,Planilha1!A:C,3,0)</f>
+        <v>\d+[,.]\d{2}\b</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="6" t="str">
+        <f>VLOOKUP(A8,Planilha1!A:C,3,0)</f>
+        <v>.+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="str">
+        <f>VLOOKUP(A9,Planilha1!A:C,3,0)</f>
+        <v>[A-Z]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="6" t="str">
+        <f>VLOOKUP(A10,Planilha1!A:C,3,0)</f>
+        <v>^[a-zA-Z\u00C0-\u00FF 0-9\-\—\–]*$</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="str">
+        <f>VLOOKUP(A11,Planilha1!A:C,3,0)</f>
+        <v>[\']+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="6" t="str">
+        <f>VLOOKUP(A12,Planilha1!A:C,3,0)</f>
+        <v>\b(?:o(s)?|a(s)?|um(a)?(s)?|uns)\b|\b(?:O(s)?|A(s)?|Um(a)?(s)?|Uns)\b</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f>VLOOKUP(A13,Planilha1!A:C,3,0)</f>
+        <v>(?P&lt;hours&gt;0?[0-9]|1[0-9]|2[0-3]):(?P&lt;minutes&gt;60|[0-5][0-9]):(?P&lt;seconds&gt;60|[0-5][0-9])</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6" t="str">
+        <f>VLOOKUP(A14,Planilha1!A:C,3,0)</f>
+        <v>(?:([0-9]{1,2})([/.\-])([0-9]{1,2})\2([0-9]{4}))</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f>VLOOKUP(A15,Planilha1!A:C,3,0)</f>
+        <v>Não se aplica</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="6" t="str">
+        <f>VLOOKUP(A16,Planilha1!A:C,3,0)</f>
+        <v>\b\w+[sS]\b</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f>VLOOKUP(A17,Planilha1!A:C,3,0)</f>
+        <v>\b\d{4}\s*-\s*\d{4}\b</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="6" t="str">
+        <f>VLOOKUP(A18,Planilha1!A:C,3,0)</f>
+        <v>[0-9][,\.]</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C18" xr:uid="{1768680F-ADC9-4FEC-9480-0C381EAC24E4}"/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E6700A-990C-466A-81B3-1F77E72566F6}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,308 +1259,308 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -959,216 +1571,216 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1768680F-ADC9-4FEC-9480-0C381EAC24E4}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C890B159-C7C9-4BD1-846C-34632F268B80}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>6</v>
+      <c r="C2" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
+      <c r="C5" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>20</v>
+      <c r="C8" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalização do relatório final
</commit_message>
<xml_diff>
--- a/data/fontes/Base_Regex.xlsx
+++ b/data/fontes/Base_Regex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeil\Documents\GitHub\DataQ-culture\data\fontes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA8C7B-C62E-4837-9A12-48F14FF32073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667233A0-8569-419B-956E-C28C56242D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="4440" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="83">
   <si>
     <t>Nome da Regra</t>
   </si>
@@ -256,6 +256,33 @@
   </si>
   <si>
     <t>\b\d{4}\s*-\s*\d{4}\b</t>
+  </si>
+  <si>
+    <t>Capitalizar as inicais de nomes próprios e da primeira palavra, para outros termos use letras minúsculas</t>
+  </si>
+  <si>
+    <t>,Measurements, Measurements_Altura, Measurements_Largura, Measurements_Profundidade, Measurements_Diametro, Measurements_Peso, Measurements_Espessura,</t>
+  </si>
+  <si>
+    <t>,Class,Creation Location,Creator,Description,Location,Materials and Techniques,Other Descriptive Notes,Title,Work Type,</t>
+  </si>
+  <si>
+    <t>,Class,Creation Location,Creator,Inscription,Location,Materials and Techniques,Measurements, Measurements_Altura, Measurements_Largura, Measurements_Profundidade, Measurements_Diametro, Measurements_Peso, Measurements_Espessura,Physical Description,Work Type,Inscription,Location,</t>
+  </si>
+  <si>
+    <t>,Creator,Inscription,Materials and Techniques,Measurements, Measurements_Altura, Measurements_Largura, Measurements_Profundidade, Measurements_Diametro, Measurements_Peso,Measurements_Espessura,Work Type,Title,Date,Location,</t>
+  </si>
+  <si>
+    <t>,Class,Materials and Techniques,Work Type,</t>
+  </si>
+  <si>
+    <t>Seguir padrão para registro de horas, minutos e segundos</t>
+  </si>
+  <si>
+    <t>Seguir padrão para registro de dia, mês e ano da data</t>
+  </si>
+  <si>
+    <t>Anos com menos de 4 digitos, inserir 0 à esquerda</t>
   </si>
 </sst>
 </file>
@@ -676,13 +703,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1593F18-74CB-49B4-852F-BA4F8ACE44E1}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="74" style="9" customWidth="1"/>
     <col min="2" max="2" width="81.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -710,7 +737,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>60</v>
@@ -724,7 +751,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
@@ -739,9 +766,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -761,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>62</v>
@@ -778,7 +805,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -795,7 +822,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>63</v>
@@ -812,7 +839,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>65</v>
@@ -829,7 +856,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>66</v>
@@ -892,9 +919,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>43</v>
@@ -909,9 +936,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>43</v>
@@ -948,7 +975,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>72</v>
@@ -982,7 +1009,7 @@
         <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>39</v>
@@ -1050,9 +1077,9 @@
       <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="6" t="str">
+      <c r="C3" s="6" t="e">
         <f>VLOOKUP(A3,Planilha1!A:C,3,0)</f>
-        <v>\b\d{4}\b</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1062,9 +1089,9 @@
       <c r="B4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="6" t="str">
+      <c r="C4" s="6" t="e">
         <f>VLOOKUP(A4,Planilha1!A:C,3,0)</f>
-        <v>^([A-Z0-9]){1}(.)*</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1139,7 +1166,7 @@
         <v>^[a-zA-Z\u00C0-\u00FF 0-9\-\—\–]*$</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1170,9 +1197,9 @@
       <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="6" t="str">
+      <c r="C13" s="6" t="e">
         <f>VLOOKUP(A13,Planilha1!A:C,3,0)</f>
-        <v>(?P&lt;hours&gt;0?[0-9]|1[0-9]|2[0-3]):(?P&lt;minutes&gt;60|[0-5][0-9]):(?P&lt;seconds&gt;60|[0-5][0-9])</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1182,9 +1209,9 @@
       <c r="B14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="6" t="str">
+      <c r="C14" s="6" t="e">
         <f>VLOOKUP(A14,Planilha1!A:C,3,0)</f>
-        <v>(?:([0-9]{1,2})([/.\-])([0-9]{1,2})\2([0-9]{4}))</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1199,7 +1226,7 @@
         <v>Não se aplica</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>

</xml_diff>